<commit_message>
update ui and css
</commit_message>
<xml_diff>
--- a/data/dataset description.xlsx
+++ b/data/dataset description.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flights-analytics\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Flights_Analytics_R_Shiny\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="6648" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="6648" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset description" sheetId="1" r:id="rId1"/>
@@ -1113,6 +1113,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1221,6 +1224,51 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1251,51 +1299,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1303,9 +1306,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1640,7 +1640,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1651,7 +1651,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1660,7 +1660,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1678,7 +1678,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1687,7 +1687,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1705,7 +1705,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1723,7 +1723,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1732,7 +1732,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1743,7 +1743,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1752,7 +1752,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1790,7 +1790,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1799,7 +1799,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1808,7 +1808,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1837,7 +1837,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
@@ -1846,7 +1846,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
@@ -1855,7 +1855,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1866,7 +1866,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
@@ -1875,7 +1875,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1884,7 +1884,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
@@ -1893,7 +1893,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1904,7 +1904,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
@@ -1913,7 +1913,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="3" t="s">
         <v>31</v>
       </c>
@@ -1922,7 +1922,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="3" t="s">
         <v>32</v>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="3" t="s">
         <v>33</v>
       </c>
@@ -1970,274 +1970,274 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="18" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="20" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
     </row>
     <row r="5" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
     </row>
     <row r="7" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
     </row>
     <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="9" spans="1:15" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
     </row>
     <row r="10" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="17" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2283,154 +2283,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="39" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="39" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="40"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="39">
+      <c r="B2" s="43"/>
+      <c r="C2" s="40">
         <v>1.2</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="39">
+      <c r="D2" s="41"/>
+      <c r="E2" s="40">
         <v>1.2</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="39">
+      <c r="F2" s="41"/>
+      <c r="G2" s="40">
         <v>1.2</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2472,163 +2472,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="39" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="39" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="40"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="64">
+      <c r="B2" s="43"/>
+      <c r="C2" s="55">
         <v>1.2</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="39">
+      <c r="D2" s="56"/>
+      <c r="E2" s="40">
         <v>1.2</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="39">
+      <c r="F2" s="41"/>
+      <c r="G2" s="40">
         <v>1.2</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="66" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="71"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="71"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="71"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="71"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:D6"/>
+    <mergeCell ref="B7:D10"/>
     <mergeCell ref="B11:H12"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
@@ -2637,12 +2643,6 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="E3:H10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:D6"/>
-    <mergeCell ref="B7:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2654,7 +2654,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2668,158 +2668,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="75" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="69" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="71"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
     </row>
     <row r="11" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B3:D10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="E7:H10"/>
-    <mergeCell ref="E3:H6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
@@ -2828,6 +2821,13 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="E7:H10"/>
+    <mergeCell ref="E3:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2839,8 +2839,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2853,158 +2853,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="39" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="39" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="40"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="64">
+      <c r="B2" s="43"/>
+      <c r="C2" s="55">
         <v>1.2</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="39">
+      <c r="D2" s="56"/>
+      <c r="E2" s="40">
         <v>1.2</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="39">
+      <c r="F2" s="41"/>
+      <c r="G2" s="40">
         <v>1.2</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="66" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="71"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
     </row>
     <row r="5" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="71"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="71"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="71"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
     </row>
     <row r="11" spans="1:8" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="77"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>